<commit_message>
Add Mfr SPQ column (M) to original LAM NewParts file from BOM data
</commit_message>
<xml_diff>
--- a/Trading Analysis/LAM review/Copy of Lam-Astute_NewParts - 02122026.xlsx
+++ b/Trading Analysis/LAM review/Copy of Lam-Astute_NewParts - 02122026.xlsx
@@ -154,7 +154,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="29">
+  <cellXfs count="30">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
@@ -218,6 +218,7 @@
     <xf numFmtId="167" fontId="3" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="169" fontId="9" fillId="7" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="169" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -753,7 +754,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:L348"/>
+  <dimension ref="A1:M348"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="B17" sqref="B17"/>
@@ -773,6 +774,7 @@
     <col width="13.85546875" bestFit="1" customWidth="1" min="10" max="10"/>
     <col width="14.140625" bestFit="1" customWidth="1" min="11" max="11"/>
     <col width="16" customWidth="1" min="12" max="12"/>
+    <col width="10" customWidth="1" min="13" max="13"/>
   </cols>
   <sheetData>
     <row r="1" ht="47.25" customFormat="1" customHeight="1" s="21">
@@ -837,6 +839,11 @@
           <t>Total Difference</t>
         </is>
       </c>
+      <c r="M1" s="22" t="inlineStr">
+        <is>
+          <t>Mfr SPQ</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" s="14" t="inlineStr">
@@ -872,6 +879,9 @@
       <c r="I2" s="11" t="n"/>
       <c r="J2" s="14" t="n"/>
       <c r="K2" s="14" t="n"/>
+      <c r="M2" s="29" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="3">
       <c r="A3" s="14" t="inlineStr">
@@ -916,6 +926,9 @@
       <c r="L3" s="25" t="n">
         <v>-0.962</v>
       </c>
+      <c r="M3" s="29" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="4">
       <c r="A4" s="3" t="inlineStr">
@@ -960,6 +973,9 @@
       <c r="L4" s="25" t="n">
         <v>-5.5264</v>
       </c>
+      <c r="M4" s="29" t="n">
+        <v>1800</v>
+      </c>
     </row>
     <row r="5">
       <c r="A5" s="14" t="inlineStr">
@@ -1004,6 +1020,9 @@
       <c r="L5" s="25" t="n">
         <v>-67.7059</v>
       </c>
+      <c r="M5" s="29" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="6">
       <c r="A6" s="14" t="inlineStr">
@@ -1048,6 +1067,9 @@
       <c r="L6" s="25" t="n">
         <v>-11.3315</v>
       </c>
+      <c r="M6" s="29" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="7">
       <c r="A7" s="14" t="inlineStr">
@@ -1092,6 +1114,9 @@
       <c r="L7" s="27" t="n">
         <v>0.311</v>
       </c>
+      <c r="M7" s="29" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="8">
       <c r="A8" s="14" t="inlineStr">
@@ -1135,6 +1160,9 @@
       </c>
       <c r="L8" s="25" t="n">
         <v>-772.8506</v>
+      </c>
+      <c r="M8" s="29" t="n">
+        <v>1</v>
       </c>
     </row>
     <row r="9">
@@ -1219,6 +1247,9 @@
       <c r="L10" s="25" t="n">
         <v>-0.9101</v>
       </c>
+      <c r="M10" s="29" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="11">
       <c r="A11" s="3" t="inlineStr">
@@ -1263,6 +1294,9 @@
       <c r="L11" s="25" t="n">
         <v>-73.1048</v>
       </c>
+      <c r="M11" s="29" t="n">
+        <v>100</v>
+      </c>
     </row>
     <row r="12">
       <c r="A12" s="14" t="inlineStr">
@@ -1307,6 +1341,9 @@
       <c r="L12" s="25" t="n">
         <v>-2.0346</v>
       </c>
+      <c r="M12" s="29" t="n">
+        <v>250</v>
+      </c>
     </row>
     <row r="13">
       <c r="A13" s="14" t="inlineStr">
@@ -1351,6 +1388,9 @@
       <c r="L13" s="25" t="n">
         <v>-48.3472</v>
       </c>
+      <c r="M13" s="29" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="14">
       <c r="A14" s="14" t="inlineStr">
@@ -1395,6 +1435,9 @@
       <c r="L14" s="25" t="n">
         <v>-23.1593</v>
       </c>
+      <c r="M14" s="29" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="15">
       <c r="A15" s="3" t="inlineStr">
@@ -1439,6 +1482,9 @@
       <c r="L15" s="25" t="n">
         <v>-6.6934</v>
       </c>
+      <c r="M15" s="29" t="n">
+        <v>50</v>
+      </c>
     </row>
     <row r="16">
       <c r="A16" s="14" t="inlineStr">
@@ -1482,6 +1528,9 @@
       </c>
       <c r="L16" s="25" t="n">
         <v>-15.1619</v>
+      </c>
+      <c r="M16" s="29" t="n">
+        <v>1</v>
       </c>
     </row>
     <row r="17">
@@ -1566,6 +1615,9 @@
       <c r="L18" s="25" t="n">
         <v>-3.3922</v>
       </c>
+      <c r="M18" s="29" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="19">
       <c r="A19" s="14" t="inlineStr">
@@ -1610,6 +1662,9 @@
       <c r="L19" s="27" t="n">
         <v>2.6001</v>
       </c>
+      <c r="M19" s="29" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="20">
       <c r="A20" s="3" t="inlineStr">
@@ -1654,6 +1709,9 @@
       <c r="L20" s="25" t="n">
         <v>-119.9221</v>
       </c>
+      <c r="M20" s="29" t="n">
+        <v>30</v>
+      </c>
     </row>
     <row r="21">
       <c r="A21" s="14" t="inlineStr">
@@ -1698,6 +1756,9 @@
       <c r="L21" s="25" t="n">
         <v>-1.8143</v>
       </c>
+      <c r="M21" s="29" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="22">
       <c r="A22" s="14" t="inlineStr">
@@ -1741,6 +1802,9 @@
       </c>
       <c r="L22" s="25" t="n">
         <v>-3.3291</v>
+      </c>
+      <c r="M22" s="29" t="n">
+        <v>1</v>
       </c>
     </row>
     <row r="23">
@@ -2045,6 +2109,9 @@
       <c r="L29" s="25" t="n">
         <v>-2.1169</v>
       </c>
+      <c r="M29" s="29" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="30">
       <c r="A30" s="14" t="inlineStr">
@@ -2089,6 +2156,9 @@
       <c r="L30" s="25" t="n">
         <v>-0.5072</v>
       </c>
+      <c r="M30" s="29" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="31">
       <c r="A31" s="14" t="inlineStr">
@@ -2133,6 +2203,9 @@
       <c r="L31" s="25" t="n">
         <v>-18.765</v>
       </c>
+      <c r="M31" s="29" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="32">
       <c r="A32" s="14" t="inlineStr">
@@ -2177,6 +2250,9 @@
       <c r="L32" s="25" t="n">
         <v>-10.8242</v>
       </c>
+      <c r="M32" s="29" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="33">
       <c r="A33" s="14" t="inlineStr">
@@ -2221,6 +2297,9 @@
       <c r="L33" s="25" t="n">
         <v>-1.0998</v>
       </c>
+      <c r="M33" s="29" t="n">
+        <v>500</v>
+      </c>
     </row>
     <row r="34">
       <c r="A34" s="14" t="inlineStr">
@@ -2265,6 +2344,9 @@
       <c r="L34" s="27" t="n">
         <v>0.426</v>
       </c>
+      <c r="M34" s="29" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="35">
       <c r="A35" s="3" t="inlineStr">
@@ -2309,6 +2391,9 @@
       <c r="L35" s="25" t="n">
         <v>-18.538</v>
       </c>
+      <c r="M35" s="29" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="36">
       <c r="A36" s="14" t="inlineStr">
@@ -2353,6 +2438,9 @@
       <c r="L36" s="25" t="n">
         <v>-11.6388</v>
       </c>
+      <c r="M36" s="29" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="37">
       <c r="A37" s="14" t="inlineStr">
@@ -2397,6 +2485,9 @@
       <c r="L37" s="27" t="n">
         <v>35.8626</v>
       </c>
+      <c r="M37" s="29" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="38">
       <c r="A38" s="14" t="inlineStr">
@@ -2441,6 +2532,9 @@
       <c r="L38" s="25" t="n">
         <v>-0.8299</v>
       </c>
+      <c r="M38" s="29" t="n">
+        <v>500</v>
+      </c>
     </row>
     <row r="39">
       <c r="A39" s="14" t="inlineStr">
@@ -2485,6 +2579,9 @@
       <c r="L39" s="25" t="n">
         <v>-1.599</v>
       </c>
+      <c r="M39" s="29" t="n">
+        <v>2500</v>
+      </c>
     </row>
     <row r="40">
       <c r="A40" s="14" t="inlineStr">
@@ -2529,6 +2626,9 @@
       <c r="L40" s="25" t="n">
         <v>-13.072</v>
       </c>
+      <c r="M40" s="29" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="41">
       <c r="A41" s="14" t="inlineStr">
@@ -2572,6 +2672,9 @@
       </c>
       <c r="L41" s="25" t="n">
         <v>-0.5618</v>
+      </c>
+      <c r="M41" s="29" t="n">
+        <v>2500</v>
       </c>
     </row>
     <row r="42">
@@ -2656,6 +2759,9 @@
       <c r="L43" s="25" t="n">
         <v>-3.3264</v>
       </c>
+      <c r="M43" s="29" t="n">
+        <v>500</v>
+      </c>
     </row>
     <row r="44">
       <c r="A44" s="3" t="inlineStr">
@@ -2700,6 +2806,9 @@
       <c r="L44" s="25" t="n">
         <v>-3.5447</v>
       </c>
+      <c r="M44" s="29" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="45">
       <c r="A45" s="14" t="inlineStr">
@@ -2744,6 +2853,9 @@
       <c r="L45" s="25" t="n">
         <v>-5.1138</v>
       </c>
+      <c r="M45" s="29" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="46">
       <c r="A46" s="3" t="inlineStr">
@@ -2788,6 +2900,9 @@
       <c r="L46" s="25" t="n">
         <v>-5.6233</v>
       </c>
+      <c r="M46" s="29" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="47">
       <c r="A47" s="14" t="inlineStr">
@@ -2832,6 +2947,9 @@
       <c r="L47" s="25" t="n">
         <v>-2.6935</v>
       </c>
+      <c r="M47" s="29" t="n">
+        <v>42</v>
+      </c>
     </row>
     <row r="48">
       <c r="A48" s="14" t="inlineStr">
@@ -2876,6 +2994,9 @@
       <c r="L48" s="25" t="n">
         <v>-1.1199</v>
       </c>
+      <c r="M48" s="29" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="49">
       <c r="A49" s="14" t="inlineStr">
@@ -2920,6 +3041,9 @@
       <c r="L49" s="25" t="n">
         <v>-3.8928</v>
       </c>
+      <c r="M49" s="29" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="50">
       <c r="A50" s="3" t="inlineStr">
@@ -2964,6 +3088,9 @@
       <c r="L50" s="25" t="n">
         <v>-6.4516</v>
       </c>
+      <c r="M50" s="29" t="n">
+        <v>55</v>
+      </c>
     </row>
     <row r="51">
       <c r="A51" s="14" t="inlineStr">
@@ -3008,6 +3135,9 @@
       <c r="L51" s="25" t="n">
         <v>-0.2647</v>
       </c>
+      <c r="M51" s="29" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="52">
       <c r="A52" s="14" t="inlineStr">
@@ -3052,6 +3182,9 @@
       <c r="L52" s="25" t="n">
         <v>-12.828</v>
       </c>
+      <c r="M52" s="29" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="53">
       <c r="A53" s="14" t="inlineStr">
@@ -3096,6 +3229,9 @@
       <c r="L53" s="25" t="n">
         <v>-0.4325</v>
       </c>
+      <c r="M53" s="29" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="54">
       <c r="A54" s="14" t="inlineStr">
@@ -3140,6 +3276,9 @@
       <c r="L54" s="25" t="n">
         <v>-5.3152</v>
       </c>
+      <c r="M54" s="29" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="55">
       <c r="A55" s="3" t="inlineStr">
@@ -3184,6 +3323,9 @@
       <c r="L55" s="25" t="n">
         <v>-8.877800000000001</v>
       </c>
+      <c r="M55" s="29" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="56">
       <c r="A56" s="3" t="inlineStr">
@@ -3228,6 +3370,9 @@
       <c r="L56" s="25" t="n">
         <v>-18.45</v>
       </c>
+      <c r="M56" s="29" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="57">
       <c r="A57" s="14" t="inlineStr">
@@ -3360,6 +3505,9 @@
       <c r="L59" s="25" t="n">
         <v>-1.7344</v>
       </c>
+      <c r="M59" s="29" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="60">
       <c r="A60" s="14" t="inlineStr">
@@ -3404,6 +3552,9 @@
       <c r="L60" s="25" t="n">
         <v>-3.3085</v>
       </c>
+      <c r="M60" s="29" t="n">
+        <v>400</v>
+      </c>
     </row>
     <row r="61">
       <c r="A61" s="14" t="inlineStr">
@@ -3448,6 +3599,9 @@
       <c r="L61" s="25" t="n">
         <v>-4.9918</v>
       </c>
+      <c r="M61" s="29" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="62">
       <c r="A62" s="14" t="inlineStr">
@@ -3492,6 +3646,9 @@
       <c r="L62" s="25" t="n">
         <v>-9.565300000000001</v>
       </c>
+      <c r="M62" s="29" t="n">
+        <v>150</v>
+      </c>
     </row>
     <row r="63">
       <c r="A63" s="14" t="inlineStr">
@@ -3536,6 +3693,9 @@
       <c r="L63" s="25" t="n">
         <v>-8.483000000000001</v>
       </c>
+      <c r="M63" s="29" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="64">
       <c r="A64" s="14" t="inlineStr">
@@ -3580,6 +3740,9 @@
       <c r="L64" s="27" t="n">
         <v>32.6888</v>
       </c>
+      <c r="M64" s="29" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="65">
       <c r="A65" s="3" t="inlineStr">
@@ -3624,6 +3787,9 @@
       <c r="L65" s="25" t="n">
         <v>-4.4608</v>
       </c>
+      <c r="M65" s="29" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="66">
       <c r="A66" s="3" t="inlineStr">
@@ -3668,6 +3834,9 @@
       <c r="L66" s="25" t="n">
         <v>-5.8954</v>
       </c>
+      <c r="M66" s="29" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="67">
       <c r="A67" s="14" t="inlineStr">
@@ -3711,6 +3880,9 @@
       </c>
       <c r="L67" s="25" t="n">
         <v>-0.029</v>
+      </c>
+      <c r="M67" s="29" t="n">
+        <v>1</v>
       </c>
     </row>
     <row r="68">
@@ -3795,6 +3967,9 @@
       <c r="L69" s="25" t="n">
         <v>-1.8267</v>
       </c>
+      <c r="M69" s="29" t="n">
+        <v>575</v>
+      </c>
     </row>
     <row r="70">
       <c r="A70" s="14" t="inlineStr">
@@ -3839,6 +4014,9 @@
       <c r="L70" s="25" t="n">
         <v>-1.0453</v>
       </c>
+      <c r="M70" s="29" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="71">
       <c r="A71" s="14" t="inlineStr">
@@ -3883,6 +4061,9 @@
       <c r="L71" s="25" t="n">
         <v>-1.3305</v>
       </c>
+      <c r="M71" s="29" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="72">
       <c r="A72" s="14" t="inlineStr">
@@ -3927,6 +4108,9 @@
       <c r="L72" s="25" t="n">
         <v>-1.5901</v>
       </c>
+      <c r="M72" s="29" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="73">
       <c r="A73" s="3" t="inlineStr">
@@ -3971,6 +4155,9 @@
       <c r="L73" s="25" t="n">
         <v>-0.2989</v>
       </c>
+      <c r="M73" s="29" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="74">
       <c r="A74" s="14" t="inlineStr">
@@ -4015,6 +4202,9 @@
       <c r="L74" s="25" t="n">
         <v>-0.4464</v>
       </c>
+      <c r="M74" s="29" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="75">
       <c r="A75" s="14" t="inlineStr">
@@ -4059,6 +4249,9 @@
       <c r="L75" s="25" t="n">
         <v>-4.3498</v>
       </c>
+      <c r="M75" s="29" t="n">
+        <v>500</v>
+      </c>
     </row>
     <row r="76">
       <c r="A76" s="14" t="inlineStr">
@@ -4103,6 +4296,9 @@
       <c r="L76" s="25" t="n">
         <v>-1.418</v>
       </c>
+      <c r="M76" s="29" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="77">
       <c r="A77" s="14" t="inlineStr">
@@ -4147,6 +4343,9 @@
       <c r="L77" s="25" t="n">
         <v>-6.8223</v>
       </c>
+      <c r="M77" s="29" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="78">
       <c r="A78" s="14" t="inlineStr">
@@ -4191,6 +4390,9 @@
       <c r="L78" s="25" t="n">
         <v>-1.6821</v>
       </c>
+      <c r="M78" s="29" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="79">
       <c r="A79" s="3" t="inlineStr">
@@ -4235,6 +4437,9 @@
       <c r="L79" s="25" t="n">
         <v>-9.5756</v>
       </c>
+      <c r="M79" s="29" t="n">
+        <v>2000</v>
+      </c>
     </row>
     <row r="80">
       <c r="A80" s="14" t="inlineStr">
@@ -4279,6 +4484,9 @@
       <c r="L80" s="27" t="n">
         <v>0.7726</v>
       </c>
+      <c r="M80" s="29" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="81">
       <c r="A81" s="3" t="inlineStr">
@@ -4323,6 +4531,9 @@
       <c r="L81" s="25" t="n">
         <v>-3.0185</v>
       </c>
+      <c r="M81" s="29" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="82">
       <c r="A82" s="14" t="inlineStr">
@@ -4367,6 +4578,9 @@
       <c r="L82" s="25" t="n">
         <v>-0.6288</v>
       </c>
+      <c r="M82" s="29" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="83">
       <c r="A83" s="14" t="inlineStr">
@@ -4411,6 +4625,9 @@
       <c r="L83" s="25" t="n">
         <v>-0.8572</v>
       </c>
+      <c r="M83" s="29" t="n">
+        <v>2500</v>
+      </c>
     </row>
     <row r="84">
       <c r="A84" s="14" t="inlineStr">
@@ -4455,6 +4672,9 @@
       <c r="L84" s="25" t="n">
         <v>-1.329</v>
       </c>
+      <c r="M84" s="29" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="85">
       <c r="A85" s="3" t="inlineStr">
@@ -4499,6 +4719,9 @@
       <c r="L85" s="25" t="n">
         <v>-6.4576</v>
       </c>
+      <c r="M85" s="29" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="86">
       <c r="A86" s="3" t="inlineStr">
@@ -4543,6 +4766,9 @@
       <c r="L86" s="25" t="n">
         <v>-0.8656</v>
       </c>
+      <c r="M86" s="29" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="87">
       <c r="A87" s="14" t="inlineStr">
@@ -4631,6 +4857,9 @@
       <c r="L88" s="25" t="n">
         <v>-1.6022</v>
       </c>
+      <c r="M88" s="29" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="89">
       <c r="A89" s="14" t="inlineStr">
@@ -4674,6 +4903,9 @@
       </c>
       <c r="L89" s="25" t="n">
         <v>-0.2291</v>
+      </c>
+      <c r="M89" s="29" t="n">
+        <v>5000</v>
       </c>
     </row>
     <row r="90">
@@ -4802,6 +5034,9 @@
       <c r="L92" s="25" t="n">
         <v>-3.0903</v>
       </c>
+      <c r="M92" s="29" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="93">
       <c r="A93" s="14" t="inlineStr">
@@ -4846,6 +5081,9 @@
       <c r="L93" s="25" t="n">
         <v>-0.1522</v>
       </c>
+      <c r="M93" s="29" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="94">
       <c r="A94" s="14" t="inlineStr">
@@ -4890,6 +5128,9 @@
       <c r="L94" s="25" t="n">
         <v>-0.5481</v>
       </c>
+      <c r="M94" s="29" t="n">
+        <v>5</v>
+      </c>
     </row>
     <row r="95">
       <c r="A95" s="14" t="inlineStr">
@@ -4934,6 +5175,9 @@
       <c r="L95" s="25" t="n">
         <v>-1.24</v>
       </c>
+      <c r="M95" s="29" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="96">
       <c r="A96" s="14" t="inlineStr">
@@ -4978,6 +5222,9 @@
       <c r="L96" s="25" t="n">
         <v>-0.2123</v>
       </c>
+      <c r="M96" s="29" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="97">
       <c r="A97" s="3" t="inlineStr">
@@ -5022,6 +5269,9 @@
       <c r="L97" s="25" t="n">
         <v>-6.6943</v>
       </c>
+      <c r="M97" s="29" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="98">
       <c r="A98" s="3" t="inlineStr">
@@ -5066,6 +5316,9 @@
       <c r="L98" s="25" t="n">
         <v>-21.9322</v>
       </c>
+      <c r="M98" s="29" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="99">
       <c r="A99" s="14" t="inlineStr">
@@ -5110,6 +5363,9 @@
       <c r="L99" s="25" t="n">
         <v>-0.2168</v>
       </c>
+      <c r="M99" s="29" t="n">
+        <v>1000</v>
+      </c>
     </row>
     <row r="100">
       <c r="A100" s="3" t="inlineStr">
@@ -5154,6 +5410,9 @@
       <c r="L100" s="25" t="n">
         <v>-3.2835</v>
       </c>
+      <c r="M100" s="29" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="101">
       <c r="A101" s="14" t="inlineStr">
@@ -5198,6 +5457,9 @@
       <c r="L101" s="27" t="n">
         <v>0.1225</v>
       </c>
+      <c r="M101" s="29" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="102">
       <c r="A102" s="14" t="inlineStr">
@@ -5242,6 +5504,9 @@
       <c r="L102" s="25" t="n">
         <v>-1.2505</v>
       </c>
+      <c r="M102" s="29" t="n">
+        <v>2500</v>
+      </c>
     </row>
     <row r="103">
       <c r="A103" s="14" t="inlineStr">
@@ -5286,6 +5551,9 @@
       <c r="L103" s="25" t="n">
         <v>-0.8147</v>
       </c>
+      <c r="M103" s="29" t="n">
+        <v>300</v>
+      </c>
     </row>
     <row r="104">
       <c r="A104" s="14" t="inlineStr">
@@ -5329,6 +5597,9 @@
       </c>
       <c r="L104" s="25" t="n">
         <v>-1.2192</v>
+      </c>
+      <c r="M104" s="29" t="n">
+        <v>1</v>
       </c>
     </row>
     <row r="105">
@@ -5413,6 +5684,9 @@
       <c r="L106" s="25" t="n">
         <v>-1.0771</v>
       </c>
+      <c r="M106" s="29" t="n">
+        <v>2500</v>
+      </c>
     </row>
     <row r="107">
       <c r="A107" s="14" t="inlineStr">
@@ -5457,6 +5731,9 @@
       <c r="L107" s="25" t="n">
         <v>-3.9667</v>
       </c>
+      <c r="M107" s="29" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="108">
       <c r="A108" s="14" t="inlineStr">
@@ -5501,6 +5778,9 @@
       <c r="L108" s="25" t="n">
         <v>-0.9489</v>
       </c>
+      <c r="M108" s="29" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="109">
       <c r="A109" s="3" t="inlineStr">
@@ -5545,6 +5825,9 @@
       <c r="L109" s="25" t="n">
         <v>-3.4486</v>
       </c>
+      <c r="M109" s="29" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="110">
       <c r="A110" s="14" t="inlineStr">
@@ -5589,6 +5872,9 @@
       <c r="L110" s="25" t="n">
         <v>-0.5253</v>
       </c>
+      <c r="M110" s="29" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="111">
       <c r="A111" s="3" t="inlineStr">
@@ -5633,6 +5919,9 @@
       <c r="L111" s="25" t="n">
         <v>-3.3208</v>
       </c>
+      <c r="M111" s="29" t="n">
+        <v>2000</v>
+      </c>
     </row>
     <row r="112">
       <c r="A112" s="14" t="inlineStr">
@@ -5677,6 +5966,9 @@
       <c r="L112" s="25" t="n">
         <v>-0.9601</v>
       </c>
+      <c r="M112" s="29" t="n">
+        <v>2500</v>
+      </c>
     </row>
     <row r="113">
       <c r="A113" s="14" t="inlineStr">
@@ -5721,6 +6013,9 @@
       <c r="L113" s="25" t="n">
         <v>-3.5031</v>
       </c>
+      <c r="M113" s="29" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="114">
       <c r="A114" s="14" t="inlineStr">
@@ -5809,6 +6104,9 @@
       <c r="L115" s="25" t="n">
         <v>-3.168</v>
       </c>
+      <c r="M115" s="29" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="116">
       <c r="A116" s="14" t="inlineStr">
@@ -5853,6 +6151,9 @@
       <c r="L116" s="25" t="n">
         <v>-1.0337</v>
       </c>
+      <c r="M116" s="29" t="n">
+        <v>300</v>
+      </c>
     </row>
     <row r="117">
       <c r="A117" s="3" t="inlineStr">
@@ -5897,6 +6198,9 @@
       <c r="L117" s="25" t="n">
         <v>-9.2942</v>
       </c>
+      <c r="M117" s="29" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="118">
       <c r="A118" s="14" t="inlineStr">
@@ -5941,6 +6245,9 @@
       <c r="L118" s="25" t="n">
         <v>-2.358</v>
       </c>
+      <c r="M118" s="29" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="119">
       <c r="A119" s="14" t="inlineStr">
@@ -5985,6 +6292,9 @@
       <c r="L119" s="25" t="n">
         <v>-0.4149</v>
       </c>
+      <c r="M119" s="29" t="n">
+        <v>2000</v>
+      </c>
     </row>
     <row r="120">
       <c r="A120" s="14" t="inlineStr">
@@ -6029,6 +6339,9 @@
       <c r="L120" s="25" t="n">
         <v>-0.8766</v>
       </c>
+      <c r="M120" s="29" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="121">
       <c r="A121" s="14" t="inlineStr">
@@ -6073,6 +6386,9 @@
       <c r="L121" s="25" t="n">
         <v>-2.1864</v>
       </c>
+      <c r="M121" s="29" t="n">
+        <v>94</v>
+      </c>
     </row>
     <row r="122">
       <c r="A122" s="14" t="inlineStr">
@@ -6117,6 +6433,9 @@
       <c r="L122" s="25" t="n">
         <v>-4.318</v>
       </c>
+      <c r="M122" s="29" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="123">
       <c r="A123" s="14" t="inlineStr">
@@ -6161,6 +6480,9 @@
       <c r="L123" s="25" t="n">
         <v>-2.1249</v>
       </c>
+      <c r="M123" s="29" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="124">
       <c r="A124" s="14" t="inlineStr">
@@ -6205,6 +6527,9 @@
       <c r="L124" s="25" t="n">
         <v>-0.3513</v>
       </c>
+      <c r="M124" s="29" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="125">
       <c r="A125" s="14" t="inlineStr">
@@ -6249,6 +6574,9 @@
       <c r="L125" s="25" t="n">
         <v>-0.3381</v>
       </c>
+      <c r="M125" s="29" t="n">
+        <v>1000</v>
+      </c>
     </row>
     <row r="126">
       <c r="A126" s="14" t="inlineStr">
@@ -6293,6 +6621,9 @@
       <c r="L126" s="25" t="n">
         <v>-0.5697</v>
       </c>
+      <c r="M126" s="29" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="127">
       <c r="A127" s="14" t="inlineStr">
@@ -6337,6 +6668,9 @@
       <c r="L127" s="25" t="n">
         <v>-0.3288</v>
       </c>
+      <c r="M127" s="29" t="n">
+        <v>4000</v>
+      </c>
     </row>
     <row r="128">
       <c r="A128" s="14" t="inlineStr">
@@ -6381,6 +6715,9 @@
       <c r="L128" s="27" t="n">
         <v>0.0172</v>
       </c>
+      <c r="M128" s="29" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="129">
       <c r="A129" s="14" t="inlineStr">
@@ -6425,6 +6762,9 @@
       <c r="L129" s="25" t="n">
         <v>-3.2799</v>
       </c>
+      <c r="M129" s="29" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="130">
       <c r="A130" s="14" t="inlineStr">
@@ -6469,6 +6809,9 @@
       <c r="L130" s="25" t="n">
         <v>-0.6915</v>
       </c>
+      <c r="M130" s="29" t="n">
+        <v>5000</v>
+      </c>
     </row>
     <row r="131">
       <c r="A131" s="14" t="inlineStr">
@@ -6513,6 +6856,9 @@
       <c r="L131" s="25" t="n">
         <v>-2.206</v>
       </c>
+      <c r="M131" s="29" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="132">
       <c r="A132" s="3" t="inlineStr">
@@ -6557,6 +6903,9 @@
       <c r="L132" s="25" t="n">
         <v>-0.1464</v>
       </c>
+      <c r="M132" s="29" t="n">
+        <v>3000</v>
+      </c>
     </row>
     <row r="133">
       <c r="A133" s="3" t="inlineStr">
@@ -6601,6 +6950,9 @@
       <c r="L133" s="25" t="n">
         <v>-3.5805</v>
       </c>
+      <c r="M133" s="29" t="n">
+        <v>2000</v>
+      </c>
     </row>
     <row r="134">
       <c r="A134" s="3" t="inlineStr">
@@ -6645,6 +6997,9 @@
       <c r="L134" s="25" t="n">
         <v>-2.1769</v>
       </c>
+      <c r="M134" s="29" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="135">
       <c r="A135" s="14" t="inlineStr">
@@ -6689,6 +7044,9 @@
       <c r="L135" s="25" t="n">
         <v>-3.529</v>
       </c>
+      <c r="M135" s="29" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="136">
       <c r="A136" s="14" t="inlineStr">
@@ -6733,6 +7091,9 @@
       <c r="L136" s="25" t="n">
         <v>-0.6955</v>
       </c>
+      <c r="M136" s="29" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="137">
       <c r="A137" s="14" t="inlineStr">
@@ -6777,6 +7138,9 @@
       <c r="L137" s="27" t="n">
         <v>0.8597</v>
       </c>
+      <c r="M137" s="29" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="138">
       <c r="A138" s="14" t="inlineStr">
@@ -6821,6 +7185,9 @@
       <c r="L138" s="25" t="n">
         <v>-1.7304</v>
       </c>
+      <c r="M138" s="29" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="139">
       <c r="A139" s="14" t="inlineStr">
@@ -6865,6 +7232,9 @@
       <c r="L139" s="27" t="n">
         <v>0.1108</v>
       </c>
+      <c r="M139" s="29" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="140">
       <c r="A140" s="14" t="inlineStr">
@@ -6909,6 +7279,9 @@
       <c r="L140" s="25" t="n">
         <v>-2.1919</v>
       </c>
+      <c r="M140" s="29" t="n">
+        <v>20</v>
+      </c>
     </row>
     <row r="141">
       <c r="A141" s="14" t="inlineStr">
@@ -6953,6 +7326,9 @@
       <c r="L141" s="25" t="n">
         <v>-0.4688</v>
       </c>
+      <c r="M141" s="29" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="142">
       <c r="A142" s="14" t="inlineStr">
@@ -6997,6 +7373,9 @@
       <c r="L142" s="25" t="n">
         <v>-0.2381</v>
       </c>
+      <c r="M142" s="29" t="n">
+        <v>5000</v>
+      </c>
     </row>
     <row r="143">
       <c r="A143" s="14" t="inlineStr">
@@ -7041,6 +7420,9 @@
       <c r="L143" s="25" t="n">
         <v>-0.7322</v>
       </c>
+      <c r="M143" s="29" t="n">
+        <v>1000</v>
+      </c>
     </row>
     <row r="144">
       <c r="A144" s="14" t="inlineStr">
@@ -7085,6 +7467,9 @@
       <c r="L144" s="25" t="n">
         <v>-2.3193</v>
       </c>
+      <c r="M144" s="29" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="145">
       <c r="A145" s="3" t="inlineStr">
@@ -7129,6 +7514,9 @@
       <c r="L145" s="25" t="n">
         <v>-1.3942</v>
       </c>
+      <c r="M145" s="29" t="n">
+        <v>800</v>
+      </c>
     </row>
     <row r="146">
       <c r="A146" s="14" t="inlineStr">
@@ -7173,6 +7561,9 @@
       <c r="L146" s="27" t="n">
         <v>2.0052</v>
       </c>
+      <c r="M146" s="29" t="n">
+        <v>2000</v>
+      </c>
     </row>
     <row r="147">
       <c r="A147" s="14" t="inlineStr">
@@ -7217,6 +7608,9 @@
       <c r="L147" s="25" t="n">
         <v>-0.4554</v>
       </c>
+      <c r="M147" s="29" t="n">
+        <v>2000</v>
+      </c>
     </row>
     <row r="148">
       <c r="A148" s="14" t="inlineStr">
@@ -7261,6 +7655,9 @@
       <c r="L148" s="25" t="n">
         <v>-0.7925</v>
       </c>
+      <c r="M148" s="29" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="149">
       <c r="A149" s="14" t="inlineStr">
@@ -7305,6 +7702,9 @@
       <c r="L149" s="25" t="n">
         <v>-0.9863</v>
       </c>
+      <c r="M149" s="29" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="150">
       <c r="A150" s="14" t="inlineStr">
@@ -7349,6 +7749,9 @@
       <c r="L150" s="25" t="n">
         <v>-0.3814</v>
       </c>
+      <c r="M150" s="29" t="n">
+        <v>10000</v>
+      </c>
     </row>
     <row r="151">
       <c r="A151" s="14" t="inlineStr">
@@ -7393,6 +7796,9 @@
       <c r="L151" s="25" t="n">
         <v>-4.1128</v>
       </c>
+      <c r="M151" s="29" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="152">
       <c r="A152" s="3" t="inlineStr">
@@ -7437,6 +7843,9 @@
       <c r="L152" s="25" t="n">
         <v>-2.4583</v>
       </c>
+      <c r="M152" s="29" t="n">
+        <v>178</v>
+      </c>
     </row>
     <row r="153">
       <c r="A153" s="14" t="inlineStr">
@@ -7481,6 +7890,9 @@
       <c r="L153" s="25" t="n">
         <v>-1.2993</v>
       </c>
+      <c r="M153" s="29" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="154">
       <c r="A154" s="14" t="inlineStr">
@@ -7525,6 +7937,9 @@
       <c r="L154" s="27" t="n">
         <v>2.4696</v>
       </c>
+      <c r="M154" s="29" t="n">
+        <v>400</v>
+      </c>
     </row>
     <row r="155">
       <c r="A155" s="14" t="inlineStr">
@@ -7569,6 +7984,9 @@
       <c r="L155" s="25" t="n">
         <v>-1.6987</v>
       </c>
+      <c r="M155" s="29" t="n">
+        <v>864</v>
+      </c>
     </row>
     <row r="156">
       <c r="A156" s="14" t="inlineStr">
@@ -7613,6 +8031,9 @@
       <c r="L156" s="27" t="n">
         <v>0.3671</v>
       </c>
+      <c r="M156" s="29" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="157">
       <c r="A157" s="14" t="inlineStr">
@@ -7657,6 +8078,9 @@
       <c r="L157" s="27" t="n">
         <v>0.1628</v>
       </c>
+      <c r="M157" s="29" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="158">
       <c r="A158" s="14" t="inlineStr">
@@ -7701,6 +8125,9 @@
       <c r="L158" s="25" t="n">
         <v>-0.2204</v>
       </c>
+      <c r="M158" s="29" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="159">
       <c r="A159" s="14" t="inlineStr">
@@ -7745,6 +8172,9 @@
       <c r="L159" s="25" t="n">
         <v>-0.3406</v>
       </c>
+      <c r="M159" s="29" t="n">
+        <v>5000</v>
+      </c>
     </row>
     <row r="160">
       <c r="A160" s="14" t="inlineStr">
@@ -7789,6 +8219,9 @@
       <c r="L160" s="27" t="n">
         <v>1.9986</v>
       </c>
+      <c r="M160" s="29" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="161">
       <c r="A161" s="14" t="inlineStr">
@@ -7833,6 +8266,9 @@
       <c r="L161" s="25" t="n">
         <v>-1.5267</v>
       </c>
+      <c r="M161" s="29" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="162">
       <c r="A162" s="14" t="inlineStr">
@@ -7877,6 +8313,9 @@
       <c r="L162" s="25" t="n">
         <v>-1.5052</v>
       </c>
+      <c r="M162" s="29" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="163">
       <c r="A163" s="14" t="inlineStr">
@@ -7921,6 +8360,9 @@
       <c r="L163" s="25" t="n">
         <v>-0.8774999999999999</v>
       </c>
+      <c r="M163" s="29" t="n">
+        <v>500</v>
+      </c>
     </row>
     <row r="164">
       <c r="A164" s="14" t="inlineStr">
@@ -7965,6 +8407,9 @@
       <c r="L164" s="25" t="n">
         <v>-0.5158</v>
       </c>
+      <c r="M164" s="29" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="165">
       <c r="A165" s="14" t="inlineStr">
@@ -8009,6 +8454,9 @@
       <c r="L165" s="27" t="n">
         <v>3.1169</v>
       </c>
+      <c r="M165" s="29" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="166">
       <c r="A166" s="3" t="inlineStr">
@@ -8053,6 +8501,9 @@
       <c r="L166" s="25" t="n">
         <v>-1.9014</v>
       </c>
+      <c r="M166" s="29" t="n">
+        <v>100</v>
+      </c>
     </row>
     <row r="167">
       <c r="A167" s="14" t="inlineStr">
@@ -8097,6 +8548,9 @@
       <c r="L167" s="25" t="n">
         <v>-0.7443</v>
       </c>
+      <c r="M167" s="29" t="n">
+        <v>2000</v>
+      </c>
     </row>
     <row r="168">
       <c r="A168" s="14" t="inlineStr">
@@ -8141,6 +8595,9 @@
       <c r="L168" s="25" t="n">
         <v>-0.1299</v>
       </c>
+      <c r="M168" s="29" t="n">
+        <v>10000</v>
+      </c>
     </row>
     <row r="169">
       <c r="A169" s="14" t="inlineStr">
@@ -8185,6 +8642,9 @@
       <c r="L169" s="25" t="n">
         <v>-1.4223</v>
       </c>
+      <c r="M169" s="29" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="170">
       <c r="A170" s="3" t="inlineStr">
@@ -8229,6 +8689,9 @@
       <c r="L170" s="25" t="n">
         <v>-0.4595</v>
       </c>
+      <c r="M170" s="29" t="n">
+        <v>1000</v>
+      </c>
     </row>
     <row r="171">
       <c r="A171" s="3" t="inlineStr">
@@ -8273,6 +8736,9 @@
       <c r="L171" s="27" t="n">
         <v>0.7786</v>
       </c>
+      <c r="M171" s="29" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="172">
       <c r="A172" s="3" t="inlineStr">
@@ -8317,6 +8783,9 @@
       <c r="L172" s="25" t="n">
         <v>-1.8281</v>
       </c>
+      <c r="M172" s="29" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="173">
       <c r="A173" s="14" t="inlineStr">
@@ -8361,6 +8830,9 @@
       <c r="L173" s="25" t="n">
         <v>-1.5682</v>
       </c>
+      <c r="M173" s="29" t="n">
+        <v>37</v>
+      </c>
     </row>
     <row r="174">
       <c r="A174" s="14" t="inlineStr">
@@ -8405,6 +8877,9 @@
       <c r="L174" s="25" t="n">
         <v>-1.1618</v>
       </c>
+      <c r="M174" s="29" t="n">
+        <v>2000</v>
+      </c>
     </row>
     <row r="175">
       <c r="A175" s="3" t="inlineStr">
@@ -8449,6 +8924,9 @@
       <c r="L175" s="25" t="n">
         <v>-0.4572</v>
       </c>
+      <c r="M175" s="29" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="176">
       <c r="A176" s="14" t="inlineStr">
@@ -8493,6 +8971,9 @@
       <c r="L176" s="25" t="n">
         <v>-0.1635</v>
       </c>
+      <c r="M176" s="29" t="n">
+        <v>3000</v>
+      </c>
     </row>
     <row r="177">
       <c r="A177" s="14" t="inlineStr">
@@ -8537,6 +9018,9 @@
       <c r="L177" s="25" t="n">
         <v>-2.518</v>
       </c>
+      <c r="M177" s="29" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="178">
       <c r="A178" s="3" t="inlineStr">
@@ -8581,6 +9065,9 @@
       <c r="L178" s="25" t="n">
         <v>-2.1365</v>
       </c>
+      <c r="M178" s="29" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="179">
       <c r="A179" s="14" t="inlineStr">
@@ -8625,6 +9112,9 @@
       <c r="L179" s="25" t="n">
         <v>-5.1288</v>
       </c>
+      <c r="M179" s="29" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="180">
       <c r="A180" s="3" t="inlineStr">
@@ -8669,6 +9159,9 @@
       <c r="L180" s="27" t="n">
         <v>0.0849</v>
       </c>
+      <c r="M180" s="29" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="181">
       <c r="A181" s="14" t="inlineStr">
@@ -8713,6 +9206,9 @@
       <c r="L181" s="25" t="n">
         <v>-0.5208</v>
       </c>
+      <c r="M181" s="29" t="n">
+        <v>400</v>
+      </c>
     </row>
     <row r="182">
       <c r="A182" s="3" t="inlineStr">
@@ -8757,6 +9253,9 @@
       <c r="L182" s="25" t="n">
         <v>-2.594</v>
       </c>
+      <c r="M182" s="29" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="183">
       <c r="A183" s="14" t="inlineStr">
@@ -8801,6 +9300,9 @@
       <c r="L183" s="25" t="n">
         <v>-0.6748</v>
       </c>
+      <c r="M183" s="29" t="n">
+        <v>200</v>
+      </c>
     </row>
     <row r="184">
       <c r="A184" s="3" t="inlineStr">
@@ -8845,6 +9347,9 @@
       <c r="L184" s="25" t="n">
         <v>-3.1346</v>
       </c>
+      <c r="M184" s="29" t="n">
+        <v>2500</v>
+      </c>
     </row>
     <row r="185">
       <c r="A185" s="3" t="inlineStr">
@@ -8889,6 +9394,9 @@
       <c r="L185" s="25" t="n">
         <v>-0.6355</v>
       </c>
+      <c r="M185" s="29" t="n">
+        <v>500</v>
+      </c>
     </row>
     <row r="186">
       <c r="A186" s="14" t="inlineStr">
@@ -8933,6 +9441,9 @@
       <c r="L186" s="25" t="n">
         <v>-0.3459</v>
       </c>
+      <c r="M186" s="29" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="187">
       <c r="A187" s="14" t="inlineStr">
@@ -8977,6 +9488,9 @@
       <c r="L187" s="27" t="n">
         <v>0.4229</v>
       </c>
+      <c r="M187" s="29" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="188">
       <c r="A188" s="14" t="inlineStr">
@@ -9021,6 +9535,9 @@
       <c r="L188" s="25" t="n">
         <v>-0.0286</v>
       </c>
+      <c r="M188" s="29" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="189">
       <c r="A189" s="14" t="inlineStr">
@@ -9065,6 +9582,9 @@
       <c r="L189" s="25" t="n">
         <v>-2.28</v>
       </c>
+      <c r="M189" s="29" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="190">
       <c r="A190" s="14" t="inlineStr">
@@ -9109,6 +9629,9 @@
       <c r="L190" s="25" t="n">
         <v>-0.2364</v>
       </c>
+      <c r="M190" s="29" t="n">
+        <v>3000</v>
+      </c>
     </row>
     <row r="191">
       <c r="A191" s="3" t="inlineStr">
@@ -9153,6 +9676,9 @@
       <c r="L191" s="25" t="n">
         <v>-2.287</v>
       </c>
+      <c r="M191" s="29" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="192">
       <c r="A192" s="14" t="inlineStr">
@@ -9197,6 +9723,9 @@
       <c r="L192" s="25" t="n">
         <v>-0.1326</v>
       </c>
+      <c r="M192" s="29" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="193">
       <c r="A193" s="14" t="inlineStr">
@@ -9241,6 +9770,9 @@
       <c r="L193" s="25" t="n">
         <v>-0.1986</v>
       </c>
+      <c r="M193" s="29" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="194">
       <c r="A194" s="14" t="inlineStr">
@@ -9285,6 +9817,9 @@
       <c r="L194" s="25" t="n">
         <v>-0.5789</v>
       </c>
+      <c r="M194" s="29" t="n">
+        <v>2500</v>
+      </c>
     </row>
     <row r="195">
       <c r="A195" s="14" t="inlineStr">
@@ -9329,6 +9864,9 @@
       <c r="L195" s="25" t="n">
         <v>-0.0796</v>
       </c>
+      <c r="M195" s="29" t="n">
+        <v>2000</v>
+      </c>
     </row>
     <row r="196">
       <c r="A196" s="14" t="inlineStr">
@@ -9373,6 +9911,9 @@
       <c r="L196" s="25" t="n">
         <v>-0.4069</v>
       </c>
+      <c r="M196" s="29" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="197">
       <c r="A197" s="3" t="inlineStr">
@@ -9417,6 +9958,9 @@
       <c r="L197" s="25" t="n">
         <v>-1.312</v>
       </c>
+      <c r="M197" s="29" t="n">
+        <v>23</v>
+      </c>
     </row>
     <row r="198">
       <c r="A198" s="3" t="inlineStr">
@@ -9461,6 +10005,9 @@
       <c r="L198" s="25" t="n">
         <v>-0.0936</v>
       </c>
+      <c r="M198" s="29" t="n">
+        <v>1000</v>
+      </c>
     </row>
     <row r="199">
       <c r="A199" s="14" t="inlineStr">
@@ -9505,6 +10052,9 @@
       <c r="L199" s="25" t="n">
         <v>-2.9765</v>
       </c>
+      <c r="M199" s="29" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="200">
       <c r="A200" s="14" t="inlineStr">
@@ -9549,6 +10099,9 @@
       <c r="L200" s="25" t="n">
         <v>-0.4273</v>
       </c>
+      <c r="M200" s="29" t="n">
+        <v>2000</v>
+      </c>
     </row>
     <row r="201">
       <c r="A201" s="3" t="inlineStr">
@@ -9593,6 +10146,9 @@
       <c r="L201" s="25" t="n">
         <v>-0.2467</v>
       </c>
+      <c r="M201" s="29" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="202">
       <c r="A202" s="14" t="inlineStr">
@@ -9637,6 +10193,9 @@
       <c r="L202" s="25" t="n">
         <v>-1.058</v>
       </c>
+      <c r="M202" s="29" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="203">
       <c r="A203" s="14" t="inlineStr">
@@ -9681,6 +10240,9 @@
       <c r="L203" s="25" t="n">
         <v>-1.405</v>
       </c>
+      <c r="M203" s="29" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="204">
       <c r="A204" s="14" t="inlineStr">
@@ -9725,6 +10287,9 @@
       <c r="L204" s="25" t="n">
         <v>-0.2142</v>
       </c>
+      <c r="M204" s="29" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="205">
       <c r="A205" s="3" t="inlineStr">
@@ -9769,6 +10334,9 @@
       <c r="L205" s="25" t="n">
         <v>-1.79</v>
       </c>
+      <c r="M205" s="29" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="206">
       <c r="A206" s="3" t="inlineStr">
@@ -9813,6 +10381,9 @@
       <c r="L206" s="25" t="n">
         <v>-0.5197000000000001</v>
       </c>
+      <c r="M206" s="29" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="207">
       <c r="A207" s="14" t="inlineStr">
@@ -9857,6 +10428,9 @@
       <c r="L207" s="25" t="n">
         <v>-0.35</v>
       </c>
+      <c r="M207" s="29" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="208">
       <c r="A208" s="14" t="inlineStr">
@@ -9901,6 +10475,9 @@
       <c r="L208" s="25" t="n">
         <v>-0.0018</v>
       </c>
+      <c r="M208" s="29" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="209">
       <c r="A209" s="14" t="inlineStr">
@@ -9945,6 +10522,9 @@
       <c r="L209" s="25" t="n">
         <v>-0.3334</v>
       </c>
+      <c r="M209" s="29" t="n">
+        <v>100</v>
+      </c>
     </row>
     <row r="210">
       <c r="A210" s="3" t="inlineStr">
@@ -9989,6 +10569,9 @@
       <c r="L210" s="25" t="n">
         <v>-1.4923</v>
       </c>
+      <c r="M210" s="29" t="n">
+        <v>3000</v>
+      </c>
     </row>
     <row r="211">
       <c r="A211" s="14" t="inlineStr">
@@ -10033,6 +10616,9 @@
       <c r="L211" s="25" t="n">
         <v>-0.2036</v>
       </c>
+      <c r="M211" s="29" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="212">
       <c r="A212" s="14" t="inlineStr">
@@ -10077,6 +10663,9 @@
       <c r="L212" s="25" t="n">
         <v>-0.8672</v>
       </c>
+      <c r="M212" s="29" t="n">
+        <v>1500</v>
+      </c>
     </row>
     <row r="213">
       <c r="A213" s="3" t="inlineStr">
@@ -10121,6 +10710,9 @@
       <c r="L213" s="27" t="n">
         <v>0.0289</v>
       </c>
+      <c r="M213" s="29" t="n">
+        <v>5400</v>
+      </c>
     </row>
     <row r="214">
       <c r="A214" s="14" t="inlineStr">
@@ -10165,6 +10757,9 @@
       <c r="L214" s="25" t="n">
         <v>-0.1091</v>
       </c>
+      <c r="M214" s="29" t="n">
+        <v>75</v>
+      </c>
     </row>
     <row r="215">
       <c r="A215" s="3" t="inlineStr">
@@ -10209,6 +10804,9 @@
       <c r="L215" s="25" t="n">
         <v>-0.2884</v>
       </c>
+      <c r="M215" s="29" t="n">
+        <v>1200</v>
+      </c>
     </row>
     <row r="216">
       <c r="A216" s="14" t="inlineStr">
@@ -10253,6 +10851,9 @@
       <c r="L216" s="25" t="n">
         <v>-0.4217</v>
       </c>
+      <c r="M216" s="29" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="217">
       <c r="A217" s="14" t="inlineStr">
@@ -10297,6 +10898,9 @@
       <c r="L217" s="27" t="n">
         <v>0.727</v>
       </c>
+      <c r="M217" s="29" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="218">
       <c r="A218" s="14" t="inlineStr">
@@ -10341,6 +10945,9 @@
       <c r="L218" s="25" t="n">
         <v>-1.5703</v>
       </c>
+      <c r="M218" s="29" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="219">
       <c r="A219" s="14" t="inlineStr">
@@ -10385,6 +10992,9 @@
       <c r="L219" s="25" t="n">
         <v>-0.1371</v>
       </c>
+      <c r="M219" s="29" t="n">
+        <v>1000</v>
+      </c>
     </row>
     <row r="220">
       <c r="A220" s="14" t="inlineStr">
@@ -10429,6 +11039,9 @@
       <c r="L220" s="25" t="n">
         <v>-0.0319</v>
       </c>
+      <c r="M220" s="29" t="n">
+        <v>3000</v>
+      </c>
     </row>
     <row r="221">
       <c r="A221" s="14" t="inlineStr">
@@ -10473,6 +11086,9 @@
       <c r="L221" s="25" t="n">
         <v>-0.1616</v>
       </c>
+      <c r="M221" s="29" t="n">
+        <v>4000</v>
+      </c>
     </row>
     <row r="222">
       <c r="A222" s="14" t="inlineStr">
@@ -10517,6 +11133,9 @@
       <c r="L222" s="25" t="n">
         <v>-0.2482</v>
       </c>
+      <c r="M222" s="29" t="n">
+        <v>10000</v>
+      </c>
     </row>
     <row r="223">
       <c r="A223" s="14" t="inlineStr">
@@ -10561,6 +11180,9 @@
       <c r="L223" s="25" t="n">
         <v>-0.1809</v>
       </c>
+      <c r="M223" s="29" t="n">
+        <v>50</v>
+      </c>
     </row>
     <row r="224">
       <c r="A224" s="14" t="inlineStr">
@@ -10605,6 +11227,9 @@
       <c r="L224" s="25" t="n">
         <v>-0.3506</v>
       </c>
+      <c r="M224" s="29" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="225">
       <c r="A225" s="14" t="inlineStr">
@@ -10649,6 +11274,9 @@
       <c r="L225" s="25" t="n">
         <v>-1.4109</v>
       </c>
+      <c r="M225" s="29" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="226">
       <c r="A226" s="14" t="inlineStr">
@@ -10693,6 +11321,9 @@
       <c r="L226" s="25" t="n">
         <v>-0.2291</v>
       </c>
+      <c r="M226" s="29" t="n">
+        <v>5000</v>
+      </c>
     </row>
     <row r="227">
       <c r="A227" s="14" t="inlineStr">
@@ -10737,6 +11368,9 @@
       <c r="L227" s="25" t="n">
         <v>-0.1002</v>
       </c>
+      <c r="M227" s="29" t="n">
+        <v>1100</v>
+      </c>
     </row>
     <row r="228">
       <c r="A228" s="14" t="inlineStr">
@@ -10781,6 +11415,9 @@
       <c r="L228" s="25" t="n">
         <v>-0.0554</v>
       </c>
+      <c r="M228" s="29" t="n">
+        <v>1000</v>
+      </c>
     </row>
     <row r="229">
       <c r="A229" s="14" t="inlineStr">
@@ -10825,6 +11462,9 @@
       <c r="L229" s="25" t="n">
         <v>-0.004</v>
       </c>
+      <c r="M229" s="29" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="230">
       <c r="A230" s="3" t="inlineStr">
@@ -10869,6 +11509,9 @@
       <c r="L230" s="25" t="n">
         <v>-0.387</v>
       </c>
+      <c r="M230" s="29" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="231">
       <c r="A231" s="14" t="inlineStr">
@@ -10913,6 +11556,9 @@
       <c r="L231" s="25" t="n">
         <v>-0.2211</v>
       </c>
+      <c r="M231" s="29" t="n">
+        <v>1000</v>
+      </c>
     </row>
     <row r="232">
       <c r="A232" s="14" t="inlineStr">
@@ -10957,6 +11603,9 @@
       <c r="L232" s="25" t="n">
         <v>-0.0756</v>
       </c>
+      <c r="M232" s="29" t="n">
+        <v>3000</v>
+      </c>
     </row>
     <row r="233">
       <c r="A233" s="3" t="inlineStr">
@@ -11001,6 +11650,9 @@
       <c r="L233" s="25" t="n">
         <v>-0.1082</v>
       </c>
+      <c r="M233" s="29" t="n">
+        <v>5000</v>
+      </c>
     </row>
     <row r="234">
       <c r="A234" s="14" t="inlineStr">
@@ -11045,6 +11697,9 @@
       <c r="L234" s="25" t="n">
         <v>-0.0176</v>
       </c>
+      <c r="M234" s="29" t="n">
+        <v>5000</v>
+      </c>
     </row>
     <row r="235">
       <c r="A235" s="14" t="inlineStr">
@@ -11089,6 +11744,9 @@
       <c r="L235" s="25" t="n">
         <v>-0.3645</v>
       </c>
+      <c r="M235" s="29" t="n">
+        <v>1000</v>
+      </c>
     </row>
     <row r="236">
       <c r="A236" s="14" t="inlineStr">
@@ -11133,6 +11791,9 @@
       <c r="L236" s="25" t="n">
         <v>-0.0789</v>
       </c>
+      <c r="M236" s="29" t="n">
+        <v>2000</v>
+      </c>
     </row>
     <row r="237">
       <c r="A237" s="14" t="inlineStr">
@@ -11177,6 +11838,9 @@
       <c r="L237" s="27" t="n">
         <v>0.1665</v>
       </c>
+      <c r="M237" s="29" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="238">
       <c r="A238" s="14" t="inlineStr">
@@ -11221,6 +11885,9 @@
       <c r="L238" s="25" t="n">
         <v>-0.0314</v>
       </c>
+      <c r="M238" s="29" t="n">
+        <v>3000</v>
+      </c>
     </row>
     <row r="239">
       <c r="A239" s="3" t="inlineStr">
@@ -11265,6 +11932,9 @@
       <c r="L239" s="25" t="n">
         <v>-0.1064</v>
       </c>
+      <c r="M239" s="29" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="240">
       <c r="A240" s="14" t="inlineStr">
@@ -11309,6 +11979,9 @@
       <c r="L240" s="27" t="n">
         <v>0.0262</v>
       </c>
+      <c r="M240" s="29" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="241">
       <c r="A241" s="14" t="inlineStr">
@@ -11353,6 +12026,9 @@
       <c r="L241" s="25" t="n">
         <v>-0.062</v>
       </c>
+      <c r="M241" s="29" t="n">
+        <v>1000</v>
+      </c>
     </row>
     <row r="242">
       <c r="A242" s="14" t="inlineStr">
@@ -11397,6 +12073,9 @@
       <c r="L242" s="25" t="n">
         <v>-0.1201</v>
       </c>
+      <c r="M242" s="29" t="n">
+        <v>4000</v>
+      </c>
     </row>
     <row r="243">
       <c r="A243" s="14" t="inlineStr">
@@ -11441,6 +12120,9 @@
       <c r="L243" s="25" t="n">
         <v>-0.25</v>
       </c>
+      <c r="M243" s="29" t="n">
+        <v>10000</v>
+      </c>
     </row>
     <row r="244">
       <c r="A244" s="14" t="inlineStr">
@@ -11485,6 +12167,9 @@
       <c r="L244" s="25" t="n">
         <v>-0.2822</v>
       </c>
+      <c r="M244" s="29" t="n">
+        <v>2500</v>
+      </c>
     </row>
     <row r="245">
       <c r="A245" s="14" t="inlineStr">
@@ -11529,6 +12214,9 @@
       <c r="L245" s="25" t="n">
         <v>-0.0066</v>
       </c>
+      <c r="M245" s="29" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="246">
       <c r="A246" s="14" t="inlineStr">
@@ -11573,6 +12261,9 @@
       <c r="L246" s="25" t="n">
         <v>-0.1515</v>
       </c>
+      <c r="M246" s="29" t="n">
+        <v>5000</v>
+      </c>
     </row>
     <row r="247">
       <c r="A247" s="14" t="inlineStr">
@@ -11617,6 +12308,9 @@
       <c r="L247" s="25" t="n">
         <v>-0.2357</v>
       </c>
+      <c r="M247" s="29" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="248">
       <c r="A248" s="14" t="inlineStr">
@@ -11661,6 +12355,9 @@
       <c r="L248" s="27" t="n">
         <v>0.005</v>
       </c>
+      <c r="M248" s="29" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="249">
       <c r="A249" s="3" t="inlineStr">
@@ -11705,6 +12402,9 @@
       <c r="L249" s="25" t="n">
         <v>-0.0978</v>
       </c>
+      <c r="M249" s="29" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="250">
       <c r="A250" s="14" t="inlineStr">
@@ -11749,6 +12449,9 @@
       <c r="L250" s="25" t="n">
         <v>-0.0515</v>
       </c>
+      <c r="M250" s="29" t="n">
+        <v>10000</v>
+      </c>
     </row>
     <row r="251">
       <c r="A251" s="14" t="inlineStr">
@@ -11793,6 +12496,9 @@
       <c r="L251" s="25" t="n">
         <v>-0.107</v>
       </c>
+      <c r="M251" s="29" t="n">
+        <v>2000</v>
+      </c>
     </row>
     <row r="252">
       <c r="A252" s="14" t="inlineStr">
@@ -11837,6 +12543,9 @@
       <c r="L252" s="25" t="n">
         <v>-0.0139</v>
       </c>
+      <c r="M252" s="29" t="n">
+        <v>5000</v>
+      </c>
     </row>
     <row r="253">
       <c r="A253" s="3" t="inlineStr">
@@ -11881,6 +12590,9 @@
       <c r="L253" s="25" t="n">
         <v>-0.096</v>
       </c>
+      <c r="M253" s="29" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="254">
       <c r="A254" s="14" t="inlineStr">
@@ -11925,6 +12637,9 @@
       <c r="L254" s="27" t="n">
         <v>0.0447</v>
       </c>
+      <c r="M254" s="29" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="255">
       <c r="A255" s="14" t="inlineStr">
@@ -11969,6 +12684,9 @@
       <c r="L255" s="27" t="n">
         <v>0.2617</v>
       </c>
+      <c r="M255" s="29" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="256">
       <c r="A256" s="3" t="inlineStr">
@@ -12013,6 +12731,9 @@
       <c r="L256" s="25" t="n">
         <v>-0.0984</v>
       </c>
+      <c r="M256" s="29" t="n">
+        <v>5000</v>
+      </c>
     </row>
     <row r="257">
       <c r="A257" s="14" t="inlineStr">
@@ -12057,6 +12778,9 @@
       <c r="L257" s="27" t="n">
         <v>0.1086</v>
       </c>
+      <c r="M257" s="29" t="n">
+        <v>5000</v>
+      </c>
     </row>
     <row r="258">
       <c r="A258" s="14" t="inlineStr">
@@ -12101,6 +12825,9 @@
       <c r="L258" s="25" t="n">
         <v>-0.025</v>
       </c>
+      <c r="M258" s="29" t="n">
+        <v>750</v>
+      </c>
     </row>
     <row r="259">
       <c r="A259" s="3" t="inlineStr">
@@ -12145,6 +12872,9 @@
       <c r="L259" s="25" t="n">
         <v>-0.1066</v>
       </c>
+      <c r="M259" s="29" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="260">
       <c r="A260" s="14" t="inlineStr">
@@ -12188,6 +12918,9 @@
       </c>
       <c r="L260" s="27" t="n">
         <v>0.0123</v>
+      </c>
+      <c r="M260" s="29" t="n">
+        <v>4000</v>
       </c>
     </row>
     <row r="261">
@@ -12272,6 +13005,9 @@
       <c r="L262" s="27" t="n">
         <v>42.8825</v>
       </c>
+      <c r="M262" s="29" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="263">
       <c r="A263" s="3" t="inlineStr">
@@ -12394,6 +13130,9 @@
       <c r="L265" s="25" t="n">
         <v>-0.7642</v>
       </c>
+      <c r="M265" s="29" t="n">
+        <v>5000</v>
+      </c>
     </row>
     <row r="266">
       <c r="A266" s="14" t="inlineStr">
@@ -12435,6 +13174,9 @@
       </c>
       <c r="L266" s="27" t="n">
         <v>0.4929</v>
+      </c>
+      <c r="M266" s="29" t="n">
+        <v>2000</v>
       </c>
     </row>
     <row r="267">
@@ -13074,6 +13816,9 @@
       <c r="L283" s="27" t="n">
         <v>0.0982</v>
       </c>
+      <c r="M283" s="29" t="n">
+        <v>4000</v>
+      </c>
     </row>
     <row r="284">
       <c r="A284" s="14" t="inlineStr">
@@ -13116,6 +13861,9 @@
       <c r="L284" s="27" t="n">
         <v>0.7614</v>
       </c>
+      <c r="M284" s="29" t="n">
+        <v>2500</v>
+      </c>
     </row>
     <row r="285">
       <c r="A285" s="14" t="inlineStr">
@@ -13157,6 +13905,9 @@
       </c>
       <c r="L285" s="27" t="n">
         <v>3.028</v>
+      </c>
+      <c r="M285" s="29" t="n">
+        <v>1</v>
       </c>
     </row>
     <row r="286">
@@ -13276,6 +14027,9 @@
       <c r="L288" s="27" t="n">
         <v>39.17</v>
       </c>
+      <c r="M288" s="29" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="289">
       <c r="A289" s="14" t="inlineStr">
@@ -13466,6 +14220,9 @@
       <c r="L293" s="27" t="n">
         <v>0.3295</v>
       </c>
+      <c r="M293" s="29" t="n">
+        <v>1000</v>
+      </c>
     </row>
     <row r="294">
       <c r="A294" s="14" t="inlineStr">
@@ -13915,6 +14672,9 @@
       <c r="L305" s="27" t="n">
         <v>10.1953</v>
       </c>
+      <c r="M305" s="29" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="306">
       <c r="A306" s="14" t="inlineStr">
@@ -14364,6 +15124,9 @@
       <c r="L317" s="27" t="n">
         <v>3.0936</v>
       </c>
+      <c r="M317" s="29" t="n">
+        <v>300</v>
+      </c>
     </row>
     <row r="318">
       <c r="A318" s="14" t="inlineStr">
@@ -14443,6 +15206,9 @@
       <c r="L319" s="27" t="n">
         <v>0.2585</v>
       </c>
+      <c r="M319" s="29" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="320">
       <c r="A320" s="3" t="inlineStr">
@@ -14480,6 +15246,9 @@
       <c r="K320" s="16" t="n">
         <v>0</v>
       </c>
+      <c r="M320" s="29" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="321">
       <c r="A321" s="3" t="inlineStr">
@@ -14517,6 +15286,9 @@
       <c r="K321" s="16" t="n">
         <v>0</v>
       </c>
+      <c r="M321" s="29" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="322">
       <c r="A322" s="14" t="inlineStr">
@@ -14558,6 +15330,9 @@
       </c>
       <c r="L322" s="27" t="n">
         <v>0.1975</v>
+      </c>
+      <c r="M322" s="29" t="n">
+        <v>1</v>
       </c>
     </row>
     <row r="323">
@@ -14596,6 +15371,9 @@
       <c r="K323" s="16" t="n">
         <v>0</v>
       </c>
+      <c r="M323" s="29" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="324">
       <c r="A324" s="3" t="inlineStr">
@@ -14633,6 +15411,9 @@
       <c r="K324" s="16" t="n">
         <v>0</v>
       </c>
+      <c r="M324" s="29" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="325">
       <c r="A325" s="3" t="inlineStr">
@@ -14670,6 +15451,9 @@
       <c r="K325" s="16" t="n">
         <v>0</v>
       </c>
+      <c r="M325" s="29" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="326">
       <c r="A326" s="3" t="inlineStr">
@@ -14707,6 +15491,9 @@
       <c r="K326" s="16" t="n">
         <v>0</v>
       </c>
+      <c r="M326" s="29" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="327">
       <c r="A327" s="3" t="inlineStr">
@@ -14744,6 +15531,9 @@
       <c r="K327" s="16" t="n">
         <v>0</v>
       </c>
+      <c r="M327" s="29" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="328">
       <c r="A328" s="3" t="inlineStr">
@@ -14781,6 +15571,9 @@
       <c r="K328" s="16" t="n">
         <v>0</v>
       </c>
+      <c r="M328" s="29" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="329">
       <c r="A329" s="3" t="inlineStr">
@@ -14818,6 +15611,9 @@
       <c r="K329" s="16" t="n">
         <v>0</v>
       </c>
+      <c r="M329" s="29" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="330">
       <c r="A330" s="3" t="inlineStr">
@@ -14855,6 +15651,9 @@
       <c r="K330" s="16" t="n">
         <v>0</v>
       </c>
+      <c r="M330" s="29" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="331">
       <c r="A331" s="3" t="inlineStr">
@@ -14892,6 +15691,9 @@
       <c r="K331" s="16" t="n">
         <v>0</v>
       </c>
+      <c r="M331" s="29" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="332">
       <c r="A332" s="3" t="inlineStr">
@@ -14929,6 +15731,9 @@
       <c r="K332" s="16" t="n">
         <v>0</v>
       </c>
+      <c r="M332" s="29" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="333">
       <c r="A333" s="3" t="inlineStr">
@@ -14966,6 +15771,9 @@
       <c r="K333" s="16" t="n">
         <v>0</v>
       </c>
+      <c r="M333" s="29" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="334">
       <c r="A334" s="3" t="inlineStr">
@@ -15003,6 +15811,9 @@
       <c r="K334" s="16" t="n">
         <v>0</v>
       </c>
+      <c r="M334" s="29" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="335">
       <c r="A335" s="3" t="inlineStr">
@@ -15040,6 +15851,9 @@
       <c r="K335" s="16" t="n">
         <v>0</v>
       </c>
+      <c r="M335" s="29" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="336">
       <c r="A336" s="14" t="inlineStr">
@@ -15077,6 +15891,9 @@
       <c r="K336" s="16" t="n">
         <v>0</v>
       </c>
+      <c r="M336" s="29" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="337">
       <c r="A337" s="14" t="inlineStr">
@@ -15114,6 +15931,9 @@
       <c r="K337" s="16" t="n">
         <v>0</v>
       </c>
+      <c r="M337" s="29" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="338">
       <c r="A338" s="3" t="inlineStr">
@@ -15151,6 +15971,9 @@
       <c r="K338" s="16" t="n">
         <v>0</v>
       </c>
+      <c r="M338" s="29" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="339">
       <c r="A339" s="14" t="inlineStr">
@@ -15304,6 +16127,9 @@
       <c r="L342" s="27" t="n">
         <v>0.695</v>
       </c>
+      <c r="M342" s="29" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="343">
       <c r="A343" s="3" t="inlineStr">
@@ -15341,6 +16167,9 @@
       <c r="K343" s="16" t="n">
         <v>0</v>
       </c>
+      <c r="M343" s="29" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="344">
       <c r="A344" s="14" t="inlineStr">
@@ -15378,6 +16207,9 @@
       <c r="K344" s="16" t="n">
         <v>0</v>
       </c>
+      <c r="M344" s="29" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="345">
       <c r="A345" s="3" t="inlineStr">
@@ -15415,6 +16247,9 @@
       <c r="K345" s="16" t="n">
         <v>0</v>
       </c>
+      <c r="M345" s="29" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="346">
       <c r="A346" s="3" t="inlineStr">
@@ -15452,6 +16287,9 @@
       <c r="K346" s="16" t="n">
         <v>0</v>
       </c>
+      <c r="M346" s="29" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="347">
       <c r="A347" s="14" t="inlineStr">
@@ -15489,6 +16327,9 @@
       <c r="K347" s="16" t="n">
         <v>0</v>
       </c>
+      <c r="M347" s="29" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="348">
       <c r="A348" s="14" t="inlineStr">
@@ -15530,6 +16371,9 @@
       </c>
       <c r="L348" s="27" t="n">
         <v>0.083</v>
+      </c>
+      <c r="M348" s="29" t="n">
+        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>